<commit_message>
$RPA0003_GraphSignins$ Process completed version 2
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\UiPath\RPA0003_GraphGroups\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\titansax\Documents\UiPath\RPA0003_GraphSignIns\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CF0F46-A6C9-4901-A589-8FEEA7F14E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A5587-36AD-4739-83AA-EB24CE3F1053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>